<commit_message>
changed for windows path sep
</commit_message>
<xml_diff>
--- a/hh_totalism.xlsx
+++ b/hh_totalism.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>district</t>
   </si>
@@ -37,45 +38,191 @@
     <t>bpl bal</t>
   </si>
   <si>
+    <t>Imphal East</t>
+  </si>
+  <si>
+    <t>SAB:14:278:01</t>
+  </si>
+  <si>
+    <t>urban</t>
+  </si>
+  <si>
+    <t>Imphal West</t>
+  </si>
+  <si>
+    <t>SAB:14:277:01</t>
+  </si>
+  <si>
+    <t>Thoubal</t>
+  </si>
+  <si>
+    <t>SAB:14:276:01</t>
+  </si>
+  <si>
     <t>Bishnupur</t>
   </si>
   <si>
+    <t>Bishnupur C.D.Block</t>
+  </si>
+  <si>
+    <t>rural</t>
+  </si>
+  <si>
+    <t>Moirang C.D.Block</t>
+  </si>
+  <si>
     <t>MOIRANG</t>
   </si>
   <si>
     <t>SAB:14:275:01</t>
   </si>
   <si>
-    <t>rural</t>
-  </si>
-  <si>
-    <t>urban</t>
+    <t>Chandel</t>
+  </si>
+  <si>
+    <t>Chakpikarong T.D.Block</t>
+  </si>
+  <si>
+    <t>Chandel T.D.Block</t>
+  </si>
+  <si>
+    <t>Machi T.D.Block</t>
+  </si>
+  <si>
+    <t>Tengnoupal T.D.Block</t>
+  </si>
+  <si>
+    <t>Churachandpur</t>
+  </si>
+  <si>
+    <t>Henglep</t>
+  </si>
+  <si>
+    <t>Singngat</t>
+  </si>
+  <si>
+    <t>Henglep T.D.Block</t>
+  </si>
+  <si>
+    <t>Lamka</t>
+  </si>
+  <si>
+    <t>Parbung T.D.Block</t>
+  </si>
+  <si>
+    <t>Samulamlan</t>
+  </si>
+  <si>
+    <t>Thanlon T.D.Block</t>
+  </si>
+  <si>
+    <t>Jiribam</t>
+  </si>
+  <si>
+    <t>Keirao Bitra</t>
+  </si>
+  <si>
+    <t>Porompat</t>
+  </si>
+  <si>
+    <t>Sawombung</t>
+  </si>
+  <si>
+    <t>Imphal West-II C.D.Block</t>
+  </si>
+  <si>
+    <t>Imphal West-I C.D.Block</t>
+  </si>
+  <si>
+    <t>IMPHAL WEST I</t>
+  </si>
+  <si>
+    <t>Senapati</t>
+  </si>
+  <si>
+    <t>Kangpokpi T.D. Block</t>
+  </si>
+  <si>
+    <t>PAOMATA</t>
+  </si>
+  <si>
+    <t>PURUL</t>
+  </si>
+  <si>
+    <t>Saikul T. D. Block</t>
+  </si>
+  <si>
+    <t>Saitu Gamphazol T.D.Block</t>
+  </si>
+  <si>
+    <t>TADUBI</t>
+  </si>
+  <si>
+    <t>Tamenglong</t>
+  </si>
+  <si>
+    <t>KHOUPUM</t>
+  </si>
+  <si>
+    <t>Nungba T.D.Block</t>
+  </si>
+  <si>
+    <t>Tamei T.D.Block</t>
+  </si>
+  <si>
+    <t>Tamenglong T.D.Block</t>
+  </si>
+  <si>
+    <t>Tousem T.D. Block</t>
+  </si>
+  <si>
+    <t>KAKCHING</t>
+  </si>
+  <si>
+    <t>LILONG</t>
+  </si>
+  <si>
+    <t>THOUBAL</t>
+  </si>
+  <si>
+    <t>Ukhrul</t>
+  </si>
+  <si>
+    <t>Chingai T.D.Block</t>
+  </si>
+  <si>
+    <t>Kamjong Chassad T.D.Block</t>
+  </si>
+  <si>
+    <t>Kasom Khullen T.D.Block</t>
+  </si>
+  <si>
+    <t>Phungyar Phaisat T.D. Block</t>
+  </si>
+  <si>
+    <t>Ukhrul T.D.Block</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,35 +237,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -406,12 +544,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
@@ -437,7 +581,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -447,48 +591,1226 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="n">
+        <v>500</v>
+      </c>
+      <c r="F2" t="n">
+        <v>150</v>
+      </c>
+      <c r="G2" t="n">
+        <v>250</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>800</v>
+      </c>
+      <c r="F3" t="n">
+        <v>240</v>
+      </c>
+      <c r="G3" t="n">
+        <v>400</v>
+      </c>
+      <c r="H3" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5235</v>
+      </c>
+      <c r="F4" t="n">
+        <v>870</v>
+      </c>
+      <c r="G4" t="n">
+        <v>760</v>
+      </c>
+      <c r="H4" t="n">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="n">
+        <v>225</v>
+      </c>
+      <c r="F5" t="n">
+        <v>185</v>
+      </c>
+      <c r="G5" t="n">
+        <v>89</v>
+      </c>
+      <c r="H5" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="n">
+        <v>9246</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1507</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3522</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="n">
         <v>7220</v>
       </c>
-      <c r="F2">
+      <c r="F7" t="n">
         <v>249</v>
       </c>
-      <c r="G2">
+      <c r="G7" t="n">
         <v>2572</v>
       </c>
-      <c r="H2">
+      <c r="H7" t="n">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E8" t="n">
+        <v>10193</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1698</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1992</v>
+      </c>
+      <c r="H8" t="n">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9221</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4305</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8954</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8905</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3902</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7440</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3754</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4899</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2409</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4628</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>10193</v>
-      </c>
-      <c r="F3">
-        <v>1698</v>
-      </c>
-      <c r="G3">
-        <v>1992</v>
-      </c>
-      <c r="H3">
-        <v>825</v>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4022</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2477</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3046</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s"/>
+      <c r="F13" t="s"/>
+      <c r="G13" t="s"/>
+      <c r="H13" t="s"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s"/>
+      <c r="F14" t="s"/>
+      <c r="G14" t="s"/>
+      <c r="H14" t="s"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2629</v>
+      </c>
+      <c r="F15" t="n">
+        <v>628</v>
+      </c>
+      <c r="G15" t="n">
+        <v>874</v>
+      </c>
+      <c r="H15" t="n">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5337</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2245</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4554</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3202</v>
+      </c>
+      <c r="F17" t="n">
+        <v>583</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="n">
+        <v>5515</v>
+      </c>
+      <c r="F18" t="n">
+        <v>953</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4028</v>
+      </c>
+      <c r="H18" t="n">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="n">
+        <v>33490</v>
+      </c>
+      <c r="F19" t="n">
+        <v>11132</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9711</v>
+      </c>
+      <c r="H19" t="n">
+        <v>5397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1882</v>
+      </c>
+      <c r="F20" t="n">
+        <v>379</v>
+      </c>
+      <c r="G20" t="n">
+        <v>427</v>
+      </c>
+      <c r="H20" t="n">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6141</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1941</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1300</v>
+      </c>
+      <c r="H21" t="n">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="n">
+        <v>7302</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1429</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2319</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="n">
+        <v>12780</v>
+      </c>
+      <c r="F23" t="n">
+        <v>821</v>
+      </c>
+      <c r="G23" t="n">
+        <v>650</v>
+      </c>
+      <c r="H23" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4545</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1007</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1777</v>
+      </c>
+      <c r="H24" t="n">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="n">
+        <v>11278</v>
+      </c>
+      <c r="F25" t="n">
+        <v>160</v>
+      </c>
+      <c r="G25" t="n">
+        <v>17</v>
+      </c>
+      <c r="H25" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="n">
+        <v>11499</v>
+      </c>
+      <c r="F26" t="n">
+        <v>517</v>
+      </c>
+      <c r="G26" t="n">
+        <v>297</v>
+      </c>
+      <c r="H26" t="n">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="n">
+        <v>11859</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3428</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1781</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="n">
+        <v>8866</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1399</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1086</v>
+      </c>
+      <c r="H28" t="n">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="n">
+        <v>12503</v>
+      </c>
+      <c r="F29" t="n">
+        <v>638</v>
+      </c>
+      <c r="G29" t="n">
+        <v>357</v>
+      </c>
+      <c r="H29" t="n">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="n">
+        <v>11182</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3710</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2819</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4335</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2083</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4684</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2797</v>
+      </c>
+      <c r="G32" t="n">
+        <v>109</v>
+      </c>
+      <c r="H32" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="n">
+        <v>5078</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3120</v>
+      </c>
+      <c r="G33" t="n">
+        <v>813</v>
+      </c>
+      <c r="H33" t="n">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="n">
+        <v>7603</v>
+      </c>
+      <c r="F34" t="n">
+        <v>5220</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3607</v>
+      </c>
+      <c r="H34" t="n">
+        <v>3504</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="n">
+        <v>22651</v>
+      </c>
+      <c r="F35" t="n">
+        <v>10709</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1904</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s"/>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="n">
+        <v>6575</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2991</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1684</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4451</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3157</v>
+      </c>
+      <c r="G38" t="n">
+        <v>499</v>
+      </c>
+      <c r="H38" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="n">
+        <v>8988</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3452</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1794</v>
+      </c>
+      <c r="H39" t="n">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" t="n">
+        <v>6652</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3238</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1189</v>
+      </c>
+      <c r="H40" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" t="n">
+        <v>13527</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2035</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1857</v>
+      </c>
+      <c r="H41" t="n">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" t="n">
+        <v>13071</v>
+      </c>
+      <c r="F42" t="n">
+        <v>3739</v>
+      </c>
+      <c r="G42" t="n">
+        <v>2053</v>
+      </c>
+      <c r="H42" t="n">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" t="n">
+        <v>18544</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4214</v>
+      </c>
+      <c r="G43" t="n">
+        <v>7580</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="n">
+        <v>5235</v>
+      </c>
+      <c r="F44" t="n">
+        <v>870</v>
+      </c>
+      <c r="G44" t="n">
+        <v>760</v>
+      </c>
+      <c r="H44" t="n">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="n">
+        <v>6101</v>
+      </c>
+      <c r="F45" t="n">
+        <v>3754</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3217</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="n">
+        <v>427</v>
+      </c>
+      <c r="F46" t="n">
+        <v>387</v>
+      </c>
+      <c r="G46" t="n">
+        <v>158</v>
+      </c>
+      <c r="H46" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="n">
+        <v>702</v>
+      </c>
+      <c r="F47" t="n">
+        <v>490</v>
+      </c>
+      <c r="G47" t="n">
+        <v>194</v>
+      </c>
+      <c r="H47" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1605</v>
+      </c>
+      <c r="F48" t="n">
+        <v>966</v>
+      </c>
+      <c r="G48" t="n">
+        <v>657</v>
+      </c>
+      <c r="H48" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" t="n">
+        <v>11137</v>
+      </c>
+      <c r="F49" t="n">
+        <v>6540</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5045</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2396</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>